<commit_message>
Funções para o classificador
</commit_message>
<xml_diff>
--- a/ROCK IN RIO.xlsx
+++ b/ROCK IN RIO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grasielly\Documents\Faculdade\2º Semestre\Cdados\P1\P1_CDados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63598bc19f8aeaea/Área de Trabalho/P1_CDados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53D6453-161D-4C3A-9A78-883D8A5508D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{C53D6453-161D-4C3A-9A78-883D8A5508D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{953D6BBC-584C-4347-A903-566CB16D4822}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1999,10 +1999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B301"/>
+  <dimension ref="A1:B302"/>
   <sheetViews>
-    <sheetView topLeftCell="A268" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B302" sqref="B302"/>
+    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A300" sqref="A300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4419,6 +4419,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B302">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4428,7 +4433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A169" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="B202" sqref="B202"/>
     </sheetView>
   </sheetViews>

</xml_diff>